<commit_message>
added:hash map in automation, record video script,date automate,read pdf script
</commit_message>
<xml_diff>
--- a/Automation/src/main/java/com/test/data/ebayTestData.xlsx
+++ b/Automation/src/main/java/com/test/data/ebayTestData.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="29">
   <si>
     <t xml:space="preserve"> firstName</t>
   </si>
@@ -204,7 +204,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -217,6 +217,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
@@ -296,7 +298,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="7:7"/>
@@ -308,7 +310,8 @@
     <col min="3" max="3" customWidth="true" hidden="false" style="0" width="27.09" collapsed="true" outlineLevel="0"/>
     <col min="4" max="5" customWidth="false" hidden="false" style="0" width="11.52" collapsed="true" outlineLevel="0"/>
     <col min="6" max="6" bestFit="true" customWidth="true" hidden="false" style="0" width="6.0703125" collapsed="true" outlineLevel="0"/>
-    <col min="7" max="1025" customWidth="false" hidden="false" style="0" width="11.52" collapsed="true" outlineLevel="0"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" hidden="false" style="0" width="6.0703125" collapsed="true" outlineLevel="0"/>
+    <col min="8" max="1025" customWidth="false" hidden="false" style="0" width="11.52" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -330,6 +333,12 @@
       <c r="F1" t="s" s="4">
         <v>27</v>
       </c>
+      <c r="G1" t="s" s="5">
+        <v>27</v>
+      </c>
+      <c r="H1" t="s" s="6">
+        <v>27</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
@@ -347,6 +356,9 @@
       <c r="F2" t="s">
         <v>28</v>
       </c>
+      <c r="G2" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
@@ -364,6 +376,9 @@
       <c r="F3" t="s">
         <v>28</v>
       </c>
+      <c r="G3" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
@@ -381,6 +396,9 @@
       <c r="F4" t="s">
         <v>28</v>
       </c>
+      <c r="G4" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
@@ -398,6 +416,9 @@
       <c r="F5" t="s">
         <v>28</v>
       </c>
+      <c r="G5" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
@@ -415,6 +436,9 @@
       <c r="F6" t="s">
         <v>28</v>
       </c>
+      <c r="G6" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
@@ -430,6 +454,9 @@
         <v>26</v>
       </c>
       <c r="F7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>